<commit_message>
clean up pyramid logic
</commit_message>
<xml_diff>
--- a/game_map_1.xlsx
+++ b/game_map_1.xlsx
@@ -1192,9 +1192,9 @@
     <row r="6" spans="1:50">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="26"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="39" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="18"/>
       <c r="I8" s="31"/>
       <c r="J8" s="25"/>
@@ -1366,7 +1366,7 @@
       <c r="D9" s="20"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
-      <c r="G9" s="10"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="31"/>
@@ -1418,7 +1418,7 @@
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>

</xml_diff>